<commit_message>
In chapter 3 cell, number and conditional formatting is covered
</commit_message>
<xml_diff>
--- a/🟢 Beginner Level (Foundations)/🎨 Chapter 3 - Formatting Essentials/Conditional formatting/Add_automatic_borders.xlsx
+++ b/🟢 Beginner Level (Foundations)/🎨 Chapter 3 - Formatting Essentials/Conditional formatting/Add_automatic_borders.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science\Self Learning\Excel\🟢 Beginner Level (Foundations)\🎨 Chapter 3 - Formatting Essentials\Conditional formatting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94DC6F60-3C4B-4152-B065-08ADB9D7D673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC5B90D-A63B-42F9-8615-0EA0F2B331AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{919BB170-2830-48BC-8DE0-7CD13C19D97C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{919BB170-2830-48BC-8DE0-7CD13C19D97C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Example 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Example 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,9 +34,74 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+  <si>
+    <t>Mohammed Jabir</t>
+  </si>
+  <si>
+    <t>Xyz</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Data Analytics</t>
+  </si>
+  <si>
+    <t>Candidate</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Hana</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>Zoya</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Lakshmi</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,16 +109,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,17 +146,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -380,12 +540,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B5C390-487F-4A5F-BFEA-C8032A00EC49}">
-  <dimension ref="A1"/>
+  <dimension ref="D2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="J13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$A$1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26200AC-950F-41EC-8F7A-27D47E2CD0D8}">
+  <dimension ref="B3:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1">
+        <v>75</v>
+      </c>
+      <c r="J4" s="1">
+        <v>63</v>
+      </c>
+      <c r="K4" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1">
+        <v>41</v>
+      </c>
+      <c r="J5" s="1">
+        <v>79</v>
+      </c>
+      <c r="K5" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1">
+        <v>94</v>
+      </c>
+      <c r="J6" s="1">
+        <v>82</v>
+      </c>
+      <c r="K6" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1">
+        <v>97</v>
+      </c>
+      <c r="J7" s="1">
+        <v>49</v>
+      </c>
+      <c r="K7" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="1">
+        <v>75</v>
+      </c>
+      <c r="J8" s="1">
+        <v>55</v>
+      </c>
+      <c r="K8" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1">
+        <v>98</v>
+      </c>
+      <c r="J9" s="1">
+        <v>91</v>
+      </c>
+      <c r="K9" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1">
+        <v>95</v>
+      </c>
+      <c r="J10" s="1">
+        <v>36</v>
+      </c>
+      <c r="K10" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1">
+        <v>97</v>
+      </c>
+      <c r="J11" s="1">
+        <v>66</v>
+      </c>
+      <c r="K11" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1">
+        <v>80</v>
+      </c>
+      <c r="J12" s="1">
+        <v>57</v>
+      </c>
+      <c r="K12" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1">
+        <v>72</v>
+      </c>
+      <c r="J13" s="1">
+        <v>45</v>
+      </c>
+      <c r="K13" s="1">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B4:E13">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B4&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>